<commit_message>
added animation and more information whilst inbooking
</commit_message>
<xml_diff>
--- a/log/661 mooie voorzitters.xlsx
+++ b/log/661 mooie voorzitters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Mollie-ID</t>
   </si>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,6 +423,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1445758</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed bug that results in files with ":" not being saved
</commit_message>
<xml_diff>
--- a/log/661 mooie voorzitters.xlsx
+++ b/log/661 mooie voorzitters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>Mollie-ID</t>
   </si>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,6 +437,118 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1445758</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1445758</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1445758</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1445758</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1445758</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1445758</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>1445758</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1445758</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated popup detetection to better work with the gives states of snelstart
</commit_message>
<xml_diff>
--- a/log/661 mooie voorzitters.xlsx
+++ b/log/661 mooie voorzitters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
   <si>
     <t>Mollie-ID</t>
   </si>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,6 +549,48 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1445758</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1445758</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1445758</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed bug that resulted in log not being found due to existance of illigal charachters
</commit_message>
<xml_diff>
--- a/log/661 mooie voorzitters.xlsx
+++ b/log/661 mooie voorzitters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>Mollie-ID</t>
   </si>
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -549,48 +549,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>1445758</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>1445758</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>1445758</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>